<commit_message>
removing colon on fastqFileName
</commit_message>
<xml_diff>
--- a/fastqFiles/fastqFiles_06.24.20.xlsx
+++ b/fastqFiles/fastqFiles_06.24.20.xlsx
@@ -91,7 +91,7 @@
     <t xml:space="preserve">Brent_large_6d_7_GTAC_7_SIC_Index2_10_AGACTGAATC_GCTTCTGT_S8_R1_001.fastq.gz</t>
   </si>
   <si>
-    <t xml:space="preserve">Brent_large_6d_8_GTAC_8_SIC_Index2_10_CTTGGAAATC_GCTTCTGT_S9_R1_001.fastq.gz:</t>
+    <t xml:space="preserve">Brent_large_6d_8_GTAC_8_SIC_Index2_10_CTTGGAAATC_GCTTCTGT_S9_R1_001.fastq.gz</t>
   </si>
   <si>
     <t xml:space="preserve">Brent_large_6d_9_GTAC_9_SIC_Index2_10_CCGATTAATC_GCTTCTGT_S10_R1_001.fastq.gz</t>
@@ -345,7 +345,7 @@
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="L:P"/>
+      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>